<commit_message>
fix invalid argument issue
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/config.xlsx
+++ b/src/test/resources/configs/config.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Calc-engine-dataTest\src\test\resources\configs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E23B73-3F80-48F7-99E0-9C83B1109077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35325" yWindow="1620" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28125" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Local</t>
   </si>
@@ -90,25 +84,46 @@
   </si>
   <si>
     <t>account</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fradow</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
   <si>
     <t>18219592968@C</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>fradow</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>password</t>
+  </si>
+  <si>
+    <t>Micorsoftaccount</t>
+  </si>
+  <si>
+    <t>fradow@163.com</t>
+  </si>
+  <si>
+    <t>Micorsofpassword</t>
+  </si>
+  <si>
+    <t>Rezie0926</t>
+  </si>
+  <si>
+    <t>baiduacc</t>
+  </si>
+  <si>
+    <t>baidupwd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +132,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -125,7 +147,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -134,36 +158,334 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="3"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <family val="3"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -171,12 +493,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -187,28 +748,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -466,26 +1070,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="13.875" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
     <col min="3" max="4" width="33.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:4">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -496,7 +1100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -507,7 +1111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -518,7 +1122,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -529,7 +1133,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -540,7 +1144,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -551,7 +1155,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -562,7 +1166,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -570,42 +1174,79 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>23</v>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" display="fradow@163.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B10" r:id="rId2" xr:uid="{8DED85BF-61EF-47CD-A359-D92A2831091E}"/>
+    <hyperlink ref="B9" r:id="rId1" display="fradow"/>
+    <hyperlink ref="B10" r:id="rId2" display="18219592968@C"/>
+    <hyperlink ref="B11" r:id="rId1" display="fradow@163.com" tooltip="mailto:fradow@163.com"/>
+    <hyperlink ref="B13" r:id="rId1" display="fradow@163.com" tooltip="mailto:fradow@163.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <sheetData/>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update hook for after each secnario and part of failed  capture generated code
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/config.xlsx
+++ b/src/test/resources/configs/config.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Local</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>baidupwd</t>
+  </si>
+  <si>
+    <t>imagepath</t>
+  </si>
+  <si>
+    <t>src/test/resources/uploadedFile/avatar.png</t>
   </si>
 </sst>
 </file>
@@ -118,12 +124,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,29 +138,51 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -162,16 +190,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -186,61 +207,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -252,6 +221,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
@@ -259,23 +268,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
@@ -283,9 +275,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -300,25 +291,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -330,55 +447,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,97 +465,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,21 +482,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -533,20 +509,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -558,6 +531,21 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -577,17 +565,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -599,10 +590,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -611,19 +602,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -632,112 +623,112 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -748,13 +739,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1076,10 +1067,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
@@ -1220,6 +1211,14 @@
       </c>
       <c r="B14" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test contributor list after rebuild
</commit_message>
<xml_diff>
--- a/src/test/resources/configs/config.xlsx
+++ b/src/test/resources/configs/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Calc-engine-dataTest\src\test\resources\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF767DE-07A2-4256-9D21-7F0D9CCA9832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7EF00F-B413-40EC-9704-EE990C220763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Local</t>
   </si>
@@ -98,35 +98,44 @@
     <t>password</t>
   </si>
   <si>
+    <t>fradow@163.com</t>
+  </si>
+  <si>
+    <t>Rezie0926</t>
+  </si>
+  <si>
+    <t>src/test/resources/uploadedFile/avatar.png</t>
+  </si>
+  <si>
+    <t>baiduAcc</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>baiduPwd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>imagePath</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>microsoftAccount</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>microsoftPassword</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>18219592968@C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>fradow@163.com</t>
-  </si>
-  <si>
-    <t>Rezie0926</t>
-  </si>
-  <si>
-    <t>src/test/resources/uploadedFile/avatar.png</t>
-  </si>
-  <si>
-    <t>baiduAcc</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>baiduPwd</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>imagePath</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>microsoftAccount</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>microsoftPassword</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEST</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -492,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -603,47 +612,55 @@
         <v>24</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -652,7 +669,7 @@
     <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B11" r:id="rId3" tooltip="mailto:fradow@163.com" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B13" r:id="rId4" tooltip="mailto:fradow@163.com" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B13" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>